<commit_message>
sobe a barra para uma diferenca de 25 seguidores!
</commit_message>
<xml_diff>
--- a/data/seguidores-por-alinhamento.xlsx
+++ b/data/seguidores-por-alinhamento.xlsx
@@ -10492,9 +10492,6 @@
       <c r="AM64">
         <v>24</v>
       </c>
-      <c r="AN64" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -10640,9 +10637,6 @@
       <c r="AM65">
         <v>23</v>
       </c>
-      <c r="AN65" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -10798,9 +10792,6 @@
       <c r="AM66">
         <v>22</v>
       </c>
-      <c r="AN66" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -10946,9 +10937,6 @@
       <c r="AM67">
         <v>22</v>
       </c>
-      <c r="AN67" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -11104,9 +11092,6 @@
       <c r="AM68">
         <v>19</v>
       </c>
-      <c r="AN68" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -11259,9 +11244,6 @@
       <c r="AM69">
         <v>18</v>
       </c>
-      <c r="AN69" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -11416,9 +11398,6 @@
       </c>
       <c r="AM70">
         <v>17</v>
-      </c>
-      <c r="AN70" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -11583,9 +11562,6 @@
       <c r="AM71">
         <v>17</v>
       </c>
-      <c r="AN71" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -11742,9 +11718,6 @@
       </c>
       <c r="AM72">
         <v>16</v>
-      </c>
-      <c r="AN72" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -11907,9 +11880,6 @@
       <c r="AM73">
         <v>16</v>
       </c>
-      <c r="AN73" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -12067,9 +12037,6 @@
       <c r="AM74">
         <v>16</v>
       </c>
-      <c r="AN74" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -12227,9 +12194,6 @@
       <c r="AM75">
         <v>16</v>
       </c>
-      <c r="AN75" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -12387,9 +12351,6 @@
       <c r="AM76">
         <v>16</v>
       </c>
-      <c r="AN76" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -12549,9 +12510,6 @@
       <c r="AM77">
         <v>16</v>
       </c>
-      <c r="AN77" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -12867,9 +12825,6 @@
       <c r="AM79">
         <v>14</v>
       </c>
-      <c r="AN79" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -13487,9 +13442,6 @@
       </c>
       <c r="AM83">
         <v>12</v>
-      </c>
-      <c r="AN83" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -13649,9 +13601,6 @@
       <c r="AM84">
         <v>11</v>
       </c>
-      <c r="AN84" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -13808,9 +13757,6 @@
       </c>
       <c r="AM85">
         <v>11</v>
-      </c>
-      <c r="AN85" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="86">

</xml_diff>